<commit_message>
Change the order of from RBG to RGB splitting
</commit_message>
<xml_diff>
--- a/Color Extractions.xlsx
+++ b/Color Extractions.xlsx
@@ -534,10 +534,10 @@
         <v>189.42937</v>
       </c>
       <c r="C2" s="1">
+        <v>101.632665</v>
+      </c>
+      <c r="D2" s="1">
         <v>87.049075</v>
-      </c>
-      <c r="D2" s="1">
-        <v>101.632665</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -548,10 +548,10 @@
         <v>149.373195</v>
       </c>
       <c r="C3" s="1">
+        <v>126.61291</v>
+      </c>
+      <c r="D3" s="1">
         <v>124.30243</v>
-      </c>
-      <c r="D3" s="1">
-        <v>126.61291</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -562,10 +562,10 @@
         <v>153.41517</v>
       </c>
       <c r="C4" s="1">
+        <v>136.499795</v>
+      </c>
+      <c r="D4" s="1">
         <v>129.97777</v>
-      </c>
-      <c r="D4" s="1">
-        <v>136.499795</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -576,10 +576,10 @@
         <v>137.122065</v>
       </c>
       <c r="C5" s="1">
+        <v>112.697615</v>
+      </c>
+      <c r="D5" s="1">
         <v>106.71553</v>
-      </c>
-      <c r="D5" s="1">
-        <v>112.697615</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -590,10 +590,10 @@
         <v>161.699585</v>
       </c>
       <c r="C6" s="1">
+        <v>140.565185</v>
+      </c>
+      <c r="D6" s="1">
         <v>138.57528</v>
-      </c>
-      <c r="D6" s="1">
-        <v>140.565185</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -604,10 +604,10 @@
         <v>130.929325</v>
       </c>
       <c r="C7" s="1">
+        <v>100.589345</v>
+      </c>
+      <c r="D7" s="1">
         <v>93.16002</v>
-      </c>
-      <c r="D7" s="1">
-        <v>100.589345</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -618,10 +618,10 @@
         <v>152.867565</v>
       </c>
       <c r="C8" s="1">
+        <v>129.696465</v>
+      </c>
+      <c r="D8" s="1">
         <v>124.46028</v>
-      </c>
-      <c r="D8" s="1">
-        <v>129.696465</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -632,10 +632,10 @@
         <v>121.76341</v>
       </c>
       <c r="C9" s="1">
+        <v>110.353325</v>
+      </c>
+      <c r="D9" s="1">
         <v>113.12934</v>
-      </c>
-      <c r="D9" s="1">
-        <v>110.353325</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -646,10 +646,10 @@
         <v>161.91819</v>
       </c>
       <c r="C10" s="1">
+        <v>122.4793</v>
+      </c>
+      <c r="D10" s="1">
         <v>109.63224</v>
-      </c>
-      <c r="D10" s="1">
-        <v>122.4793</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -660,10 +660,10 @@
         <v>147.47275</v>
       </c>
       <c r="C11" s="1">
+        <v>115.44238</v>
+      </c>
+      <c r="D11" s="1">
         <v>108.784135</v>
-      </c>
-      <c r="D11" s="1">
-        <v>115.44238</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -674,10 +674,10 @@
         <v>159.502785</v>
       </c>
       <c r="C12" s="1">
+        <v>123.590335</v>
+      </c>
+      <c r="D12" s="1">
         <v>123.36334</v>
-      </c>
-      <c r="D12" s="1">
-        <v>123.590335</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -688,10 +688,10 @@
         <v>197.92792</v>
       </c>
       <c r="C13" s="1">
+        <v>113.987485</v>
+      </c>
+      <c r="D13" s="1">
         <v>129.495265</v>
-      </c>
-      <c r="D13" s="1">
-        <v>113.987485</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -702,10 +702,10 @@
         <v>129.550885</v>
       </c>
       <c r="C14" s="1">
+        <v>98.45229</v>
+      </c>
+      <c r="D14" s="1">
         <v>94.08279</v>
-      </c>
-      <c r="D14" s="1">
-        <v>98.45229</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -716,10 +716,10 @@
         <v>121.636345</v>
       </c>
       <c r="C15" s="1">
+        <v>114.55195</v>
+      </c>
+      <c r="D15" s="1">
         <v>117.745425</v>
-      </c>
-      <c r="D15" s="1">
-        <v>114.55195</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -730,10 +730,10 @@
         <v>155.839495</v>
       </c>
       <c r="C16" s="1">
+        <v>147.371535</v>
+      </c>
+      <c r="D16" s="1">
         <v>144.651605</v>
-      </c>
-      <c r="D16" s="1">
-        <v>147.371535</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -744,10 +744,10 @@
         <v>111.65522</v>
       </c>
       <c r="C17" s="1">
+        <v>104.699</v>
+      </c>
+      <c r="D17" s="1">
         <v>106.83446</v>
-      </c>
-      <c r="D17" s="1">
-        <v>104.699</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -758,10 +758,10 @@
         <v>152.70009</v>
       </c>
       <c r="C18" s="1">
+        <v>136.77069</v>
+      </c>
+      <c r="D18" s="1">
         <v>133.617315</v>
-      </c>
-      <c r="D18" s="1">
-        <v>136.77069</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -772,10 +772,10 @@
         <v>137.38339</v>
       </c>
       <c r="C19" s="1">
+        <v>133.07438</v>
+      </c>
+      <c r="D19" s="1">
         <v>137.045425</v>
-      </c>
-      <c r="D19" s="1">
-        <v>133.07438</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -786,10 +786,10 @@
         <v>114.819245</v>
       </c>
       <c r="C20" s="1">
+        <v>89.951815</v>
+      </c>
+      <c r="D20" s="1">
         <v>87.68853</v>
-      </c>
-      <c r="D20" s="1">
-        <v>89.951815</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -800,10 +800,10 @@
         <v>125.242225</v>
       </c>
       <c r="C21" s="1">
+        <v>98.70011</v>
+      </c>
+      <c r="D21" s="1">
         <v>95.05958</v>
-      </c>
-      <c r="D21" s="1">
-        <v>98.70011</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -814,10 +814,10 @@
         <v>184.09415</v>
       </c>
       <c r="C22" s="1">
+        <v>112.86378</v>
+      </c>
+      <c r="D22" s="1">
         <v>158.182795</v>
-      </c>
-      <c r="D22" s="1">
-        <v>112.86378</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -828,10 +828,10 @@
         <v>161.160965</v>
       </c>
       <c r="C23" s="1">
+        <v>96.320995</v>
+      </c>
+      <c r="D23" s="1">
         <v>100.889825</v>
-      </c>
-      <c r="D23" s="1">
-        <v>96.320995</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -842,10 +842,10 @@
         <v>186.64742</v>
       </c>
       <c r="C24" s="1">
+        <v>107.31065</v>
+      </c>
+      <c r="D24" s="1">
         <v>158.96556</v>
-      </c>
-      <c r="D24" s="1">
-        <v>107.31065</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -856,10 +856,10 @@
         <v>121.355725</v>
       </c>
       <c r="C25" s="1">
+        <v>78.43940499999999</v>
+      </c>
+      <c r="D25" s="1">
         <v>94.000945</v>
-      </c>
-      <c r="D25" s="1">
-        <v>78.43940499999999</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -870,10 +870,10 @@
         <v>166.827435</v>
       </c>
       <c r="C26" s="1">
+        <v>121.36798</v>
+      </c>
+      <c r="D26" s="1">
         <v>136.474935</v>
-      </c>
-      <c r="D26" s="1">
-        <v>121.36798</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -884,10 +884,10 @@
         <v>148.104655</v>
       </c>
       <c r="C27" s="1">
+        <v>98.12352</v>
+      </c>
+      <c r="D27" s="1">
         <v>112.00253</v>
-      </c>
-      <c r="D27" s="1">
-        <v>98.12352</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -898,10 +898,10 @@
         <v>180.340715</v>
       </c>
       <c r="C28" s="1">
+        <v>121.426355</v>
+      </c>
+      <c r="D28" s="1">
         <v>130.12765</v>
-      </c>
-      <c r="D28" s="1">
-        <v>121.426355</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -912,10 +912,10 @@
         <v>150.337135</v>
       </c>
       <c r="C29" s="1">
+        <v>111.33515</v>
+      </c>
+      <c r="D29" s="1">
         <v>113.45072</v>
-      </c>
-      <c r="D29" s="1">
-        <v>111.33515</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -926,10 +926,10 @@
         <v>138.124075</v>
       </c>
       <c r="C30" s="1">
+        <v>109.006665</v>
+      </c>
+      <c r="D30" s="1">
         <v>112.09669</v>
-      </c>
-      <c r="D30" s="1">
-        <v>109.006665</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -940,10 +940,10 @@
         <v>128.36803</v>
       </c>
       <c r="C31" s="1">
+        <v>78.042315</v>
+      </c>
+      <c r="D31" s="1">
         <v>97.208885</v>
-      </c>
-      <c r="D31" s="1">
-        <v>78.042315</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -954,10 +954,10 @@
         <v>180.095015</v>
       </c>
       <c r="C32" s="1">
+        <v>109.532175</v>
+      </c>
+      <c r="D32" s="1">
         <v>153.708505</v>
-      </c>
-      <c r="D32" s="1">
-        <v>109.532175</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -968,10 +968,10 @@
         <v>160.16151</v>
       </c>
       <c r="C33" s="1">
+        <v>104.08952</v>
+      </c>
+      <c r="D33" s="1">
         <v>124.2288</v>
-      </c>
-      <c r="D33" s="1">
-        <v>104.08952</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -982,10 +982,10 @@
         <v>165.35091</v>
       </c>
       <c r="C34" s="1">
+        <v>95.72413</v>
+      </c>
+      <c r="D34" s="1">
         <v>135.978525</v>
-      </c>
-      <c r="D34" s="1">
-        <v>95.72413</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -996,10 +996,10 @@
         <v>181.92997</v>
       </c>
       <c r="C35" s="1">
+        <v>118.97396</v>
+      </c>
+      <c r="D35" s="1">
         <v>146.684805</v>
-      </c>
-      <c r="D35" s="1">
-        <v>118.97396</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1010,10 +1010,10 @@
         <v>195.27552</v>
       </c>
       <c r="C36" s="1">
+        <v>134.33175</v>
+      </c>
+      <c r="D36" s="1">
         <v>167.754425</v>
-      </c>
-      <c r="D36" s="1">
-        <v>134.33175</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1024,10 +1024,10 @@
         <v>174.182815</v>
       </c>
       <c r="C37" s="1">
+        <v>124.9584</v>
+      </c>
+      <c r="D37" s="1">
         <v>150.25825</v>
-      </c>
-      <c r="D37" s="1">
-        <v>124.9584</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1038,10 +1038,10 @@
         <v>173.148205</v>
       </c>
       <c r="C38" s="1">
+        <v>115.879545</v>
+      </c>
+      <c r="D38" s="1">
         <v>139.46886</v>
-      </c>
-      <c r="D38" s="1">
-        <v>115.879545</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1052,10 +1052,10 @@
         <v>172.75734</v>
       </c>
       <c r="C39" s="1">
+        <v>111.459055</v>
+      </c>
+      <c r="D39" s="1">
         <v>137.582325</v>
-      </c>
-      <c r="D39" s="1">
-        <v>111.459055</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1066,10 +1066,10 @@
         <v>170.87454</v>
       </c>
       <c r="C40" s="1">
+        <v>102.53135</v>
+      </c>
+      <c r="D40" s="1">
         <v>125.657975</v>
-      </c>
-      <c r="D40" s="1">
-        <v>102.53135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>